<commit_message>
Keyword MAtching is Successful in Test.ipynb. Will investigate using TF-IDF Vectorizer.
</commit_message>
<xml_diff>
--- a/Yeni Veri/new_processed-answers.xlsx
+++ b/Yeni Veri/new_processed-answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr codeName="BuÇalışmaKitabı"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkkas/Documents/TEZ/Tez/Yeni Veri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073EEBEA-087B-2A42-92E4-2FBFCA669E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F2584F-D722-4441-AEAD-A01420B836DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q-1" sheetId="1" r:id="rId1"/>
@@ -2292,9 +2292,6 @@
     <t>Q-1: What are some contributions of Arabs to science?</t>
   </si>
   <si>
-    <t>The Arabs made significant contributions to mathematics, astronomy, medicine, chemistry, and engineering. Notably, the development of algebra and algorithms, the optical works of Ibn al-Haytham, the medical encyclopedia "The Canon of Medicine" by Avicenna, and the contributions to trigonometry by Abū al-Wafā' are foundational. Additionally, the mathematical and astronomical works of Al-Khwarizmi are cornerstone contributions, highlighting the Arabs' role in shaping modern science.</t>
-  </si>
-  <si>
     <t>Q-2: What are the contributions of the Roman Empire to the legal system?</t>
   </si>
   <si>
@@ -2317,6 +2314,17 @@
   </si>
   <si>
     <t>The Cold War, the ideological and political rivalry that emerged between the USA and the USSR after World War II, divided the world into capitalist and communist blocs, leading to regional conflicts, arms and space races. It elevated the importance of security in international relations, led to the formation of military alliances like NATO and the Warsaw Pact, and deepened ideological divides in global politics. The end of the Cold War accelerated democratization processes in Eastern Europe and laid the groundwork for a multipolar world order.</t>
+  </si>
+  <si>
+    <t>Algebra algorithms, the optical works of Ibn al-Haytham, the medical encyclopedia "The Canon of Medicine" by Ibni Sina.  Al-Khwarizmi. Optics and theory of refraction. Lens. Accurate time measurement for pray. Direction of Mecca, Mekke.
+reflect and tranmission
+alcahol
+cartography 
+map making
+translation of greek work
+house of wisdom library
+surgery
+blood circulation</t>
   </si>
 </sst>
 </file>
@@ -2343,6 +2351,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2711,11 +2720,15 @@
   <sheetPr codeName="Sayfa1"/>
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -10027,13 +10040,14 @@
   <sheetPr codeName="Sayfa6"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="68.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="92.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -10044,44 +10058,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="176" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>754</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>755</v>
+        <v>763</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>756</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>758</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="128" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>760</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>762</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to see if this works
</commit_message>
<xml_diff>
--- a/Yeni Veri/new_processed-answers.xlsx
+++ b/Yeni Veri/new_processed-answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr codeName="BuÇalışmaKitabı"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkkas/Documents/TEZ/Tez/Yeni Veri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F2584F-D722-4441-AEAD-A01420B836DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A377E5EE-5D60-9746-87E8-9D5E32F5E9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q-1" sheetId="1" r:id="rId1"/>
@@ -2310,12 +2310,6 @@
     <t>The Industrial Revolution, originating in 18th and 19th century England, fundamentally changed the world by transitioning from manual production methods to mechanization, widespread use of coal and steam power. This era accelerated urbanization, introduced the factory system, and highlighted social class distinctions. Economic growth, population increases, and improvements in living standards were observed, alongside challenges such as labor conditions, environmental issues, and social inequities.</t>
   </si>
   <si>
-    <t>Q-5: What were the effects of the Cold War on global politics?</t>
-  </si>
-  <si>
-    <t>The Cold War, the ideological and political rivalry that emerged between the USA and the USSR after World War II, divided the world into capitalist and communist blocs, leading to regional conflicts, arms and space races. It elevated the importance of security in international relations, led to the formation of military alliances like NATO and the Warsaw Pact, and deepened ideological divides in global politics. The end of the Cold War accelerated democratization processes in Eastern Europe and laid the groundwork for a multipolar world order.</t>
-  </si>
-  <si>
     <t>Algebra algorithms, the optical works of Ibn al-Haytham, the medical encyclopedia "The Canon of Medicine" by Ibni Sina.  Al-Khwarizmi. Optics and theory of refraction. Lens. Accurate time measurement for pray. Direction of Mecca, Mekke.
 reflect and tranmission
 alcahol
@@ -2325,6 +2319,12 @@
 house of wisdom library
 surgery
 blood circulation</t>
+  </si>
+  <si>
+    <t>According to Aristotle, if a hypothesis leads to a contradiction, it must be rejected as false. This method, known as reductio ad absurdum (proof by contradiction), is used in logic to demonstrate the invalidity of an assumption by showing that it results in an impossible or contradictory outcome.</t>
+  </si>
+  <si>
+    <t>Q-5: How is a contradiction resolved in Aristotle’s logic?</t>
   </si>
 </sst>
 </file>
@@ -2720,7 +2720,7 @@
   <sheetPr codeName="Sayfa1"/>
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -8591,6 +8591,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -10040,8 +10044,8 @@
   <sheetPr codeName="Sayfa6"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10063,10 +10067,10 @@
         <v>754</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="144" x14ac:dyDescent="0.2">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>755</v>
       </c>
@@ -10074,7 +10078,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="112" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>757</v>
       </c>
@@ -10082,7 +10086,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="128" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>759</v>
       </c>
@@ -10090,9 +10094,9 @@
         <v>760</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>762</v>

</xml_diff>